<commit_message>
Review of answers some editing and interpolation
</commit_message>
<xml_diff>
--- a/Data/Delphi round 1/response sheets/Alasdair Fi - give your expert opinion on woodland condition141.xlsx
+++ b/Data/Delphi round 1/response sheets/Alasdair Fi - give your expert opinion on woodland condition141.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://woodlandtrustorg-my.sharepoint.com/personal/ewanmchenry_woodlandtrust_org_uk/Documents/WEC/Delphi round 1/response sheets/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://woodlandtrustorg-my.sharepoint.com/personal/ewanmchenry_woodlandtrust_org_uk/Documents/WEC/Woodland-condition/Data/Delphi round 1/response sheets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="815" documentId="8_{DD3140B9-43BA-428D-8B9F-F9C103859F80}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{48C5F8C4-1871-4EE0-8F0B-4701B3B79C60}"/>
+  <xr:revisionPtr revIDLastSave="820" documentId="8_{DD3140B9-43BA-428D-8B9F-F9C103859F80}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1823BE01-768A-4481-98E8-3BBB94C0CF4E}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-4815" windowWidth="16440" windowHeight="28320" firstSheet="10" activeTab="10" xr2:uid="{4926A777-5F31-4918-9802-F24A87E993EA}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" activeTab="3" xr2:uid="{4926A777-5F31-4918-9802-F24A87E993EA}"/>
   </bookViews>
   <sheets>
     <sheet name="Tree age distribution" sheetId="20" r:id="rId1"/>
@@ -4820,6 +4820,9 @@
                 <c:pt idx="2">
                   <c:v>3</c:v>
                 </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -4836,7 +4839,10 @@
                   <c:v>100</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>70</c:v>
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>100</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4864,7 +4870,7 @@
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="4"/>
-          <c:min val="0"/>
+          <c:min val="1"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
@@ -5192,38 +5198,38 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>'N tree &amp; shrub spp.'!$A$10:$A$20</c:f>
+              <c:f>'N tree &amp; shrub spp.'!$A$10:$A$19</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
-                <c:pt idx="1">
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="1">
                   <c:v>2</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="2">
                   <c:v>3</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="3">
                   <c:v>4</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="4">
                   <c:v>5</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="5">
                   <c:v>6</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="6">
                   <c:v>7</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="7">
                   <c:v>8</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="8">
                   <c:v>9</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="9">
                   <c:v>10</c:v>
                 </c:pt>
               </c:numCache>
@@ -5231,10 +5237,13 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'N tree &amp; shrub spp.'!$B$10:$B$20</c:f>
+              <c:f>'N tree &amp; shrub spp.'!$B$10:$B$19</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>100</c:v>
+                </c:pt>
                 <c:pt idx="1">
                   <c:v>100</c:v>
                 </c:pt>
@@ -5260,9 +5269,6 @@
                   <c:v>100</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>100</c:v>
-                </c:pt>
-                <c:pt idx="10">
                   <c:v>100</c:v>
                 </c:pt>
               </c:numCache>
@@ -20127,8 +20133,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0EE72529-E9AC-4265-967D-F8F100BBD70E}">
   <dimension ref="A1:R57"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -23015,7 +23021,7 @@
   <dimension ref="A1:R54"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -23144,7 +23150,7 @@
         <v>3</v>
       </c>
       <c r="B12" s="2">
-        <v>70</v>
+        <v>100</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>11</v>
@@ -23154,8 +23160,12 @@
       </c>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A13" s="2"/>
-      <c r="B13" s="2"/>
+      <c r="A13" s="2">
+        <v>4</v>
+      </c>
+      <c r="B13" s="2">
+        <v>100</v>
+      </c>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A14" s="2"/>
@@ -23531,8 +23541,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8E3BDB2-4936-4583-A0D1-731A826C7FE6}">
   <dimension ref="A1:R54"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -23607,8 +23617,12 @@
       <c r="F9" s="5"/>
     </row>
     <row r="10" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="2"/>
-      <c r="B10" s="2"/>
+      <c r="A10" s="2">
+        <v>1</v>
+      </c>
+      <c r="B10" s="2">
+        <v>100</v>
+      </c>
       <c r="D10" s="28" t="s">
         <v>10</v>
       </c>
@@ -23629,7 +23643,7 @@
     </row>
     <row r="11" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B11" s="2">
         <v>100</v>
@@ -23652,7 +23666,7 @@
     </row>
     <row r="12" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="2">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B12" s="2">
         <v>100</v>
@@ -23666,7 +23680,7 @@
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B13" s="2">
         <v>100</v>
@@ -23674,7 +23688,7 @@
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B14" s="2">
         <v>100</v>
@@ -23690,7 +23704,7 @@
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B15" s="2">
         <v>100</v>
@@ -23706,7 +23720,7 @@
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B16" s="2">
         <v>100</v>
@@ -23722,7 +23736,7 @@
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B17" s="2">
         <v>100</v>
@@ -23738,7 +23752,7 @@
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B18" s="2">
         <v>100</v>
@@ -23754,7 +23768,7 @@
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B19" s="2">
         <v>100</v>
@@ -23769,12 +23783,8 @@
       <c r="N19" s="13"/>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A20" s="2">
-        <v>10</v>
-      </c>
-      <c r="B20" s="2">
-        <v>100</v>
-      </c>
+      <c r="A20" s="2"/>
+      <c r="B20" s="2"/>
       <c r="I20" s="13" t="s">
         <v>65</v>
       </c>
@@ -26559,34 +26569,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <SharedWithUsers xmlns="cce065d8-4207-498d-8ddb-77753710233a">
-      <UserInfo>
-        <DisplayName>Christine Reid</DisplayName>
-        <AccountId>11</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Alasdair Firth</DisplayName>
-        <AccountId>30</AccountId>
-        <AccountType/>
-      </UserInfo>
-    </SharedWithUsers>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100AF102A4A1803344B8D888EB900B09227" ma:contentTypeVersion="8" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="43bc291949bcf5a898aed47fdf38e56c">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="090e8724-afd2-4a00-8d2e-c87448cad135" xmlns:ns3="cce065d8-4207-498d-8ddb-77753710233a" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="8a89575b99fa510669e25d545522f68e" ns2:_="" ns3:_="">
     <xsd:import namespace="090e8724-afd2-4a00-8d2e-c87448cad135"/>
@@ -26777,25 +26759,35 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{170C8C87-D947-4550-B837-5AF2D61371C8}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <SharedWithUsers xmlns="cce065d8-4207-498d-8ddb-77753710233a">
+      <UserInfo>
+        <DisplayName>Christine Reid</DisplayName>
+        <AccountId>11</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Alasdair Firth</DisplayName>
+        <AccountId>30</AccountId>
+        <AccountType/>
+      </UserInfo>
+    </SharedWithUsers>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{98190E4F-1B18-40B8-A20A-C34BFF97A2BB}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="cce065d8-4207-498d-8ddb-77753710233a"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E6617C3D-29D9-48EE-BF3C-21AA1A387073}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -26812,4 +26804,22 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{98190E4F-1B18-40B8-A20A-C34BFF97A2BB}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="cce065d8-4207-498d-8ddb-77753710233a"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{170C8C87-D947-4550-B837-5AF2D61371C8}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
button added for indicators in html
bit of editing to vfs in excel sheets
</commit_message>
<xml_diff>
--- a/Data/Delphi round 1/response sheets/Alasdair Fi - give your expert opinion on woodland condition141.xlsx
+++ b/Data/Delphi round 1/response sheets/Alasdair Fi - give your expert opinion on woodland condition141.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://woodlandtrustorg-my.sharepoint.com/personal/ewanmchenry_woodlandtrust_org_uk/Documents/WEC/Woodland-condition/Data/Delphi round 1/response sheets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="820" documentId="8_{DD3140B9-43BA-428D-8B9F-F9C103859F80}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1823BE01-768A-4481-98E8-3BBB94C0CF4E}"/>
+  <xr:revisionPtr revIDLastSave="827" documentId="8_{DD3140B9-43BA-428D-8B9F-F9C103859F80}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3AF0682D-6D9E-4290-9A23-E5C6CD8E14BB}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" activeTab="3" xr2:uid="{4926A777-5F31-4918-9802-F24A87E993EA}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" firstSheet="7" activeTab="13" xr2:uid="{4926A777-5F31-4918-9802-F24A87E993EA}"/>
   </bookViews>
   <sheets>
     <sheet name="Tree age distribution" sheetId="20" r:id="rId1"/>
@@ -3627,10 +3627,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>100</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>75</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>100</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3642,10 +3651,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>100</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>100</c:v>
+                  <c:v>75</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -21749,8 +21767,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A60C532-5154-4BAB-8C83-06A0BC57A749}">
   <dimension ref="A1:R57"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -21854,10 +21872,10 @@
     </row>
     <row r="13" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
+        <v>0</v>
+      </c>
+      <c r="B13" s="2">
         <v>100</v>
-      </c>
-      <c r="B13" s="2">
-        <v>0</v>
       </c>
       <c r="D13" s="28" t="s">
         <v>10</v>
@@ -21879,10 +21897,10 @@
     </row>
     <row r="14" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="2">
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="B14" s="2">
-        <v>100</v>
+        <v>75</v>
       </c>
       <c r="D14" s="28"/>
       <c r="E14" s="28"/>
@@ -21901,20 +21919,32 @@
       <c r="R14" s="28"/>
     </row>
     <row r="15" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="2"/>
-      <c r="B15" s="2"/>
+      <c r="A15" s="2">
+        <v>50</v>
+      </c>
+      <c r="B15" s="2">
+        <v>50</v>
+      </c>
       <c r="D15" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E15" s="9"/>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A16" s="2"/>
-      <c r="B16" s="2"/>
+      <c r="A16" s="2">
+        <v>75</v>
+      </c>
+      <c r="B16" s="2">
+        <v>25</v>
+      </c>
     </row>
     <row r="17" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A17" s="2"/>
-      <c r="B17" s="2"/>
+      <c r="A17" s="2">
+        <v>100</v>
+      </c>
+      <c r="B17" s="2">
+        <v>0</v>
+      </c>
       <c r="I17" s="29" t="s">
         <v>12</v>
       </c>
@@ -23541,7 +23571,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8E3BDB2-4936-4583-A0D1-731A826C7FE6}">
   <dimension ref="A1:R54"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
@@ -26569,6 +26599,34 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <SharedWithUsers xmlns="cce065d8-4207-498d-8ddb-77753710233a">
+      <UserInfo>
+        <DisplayName>Christine Reid</DisplayName>
+        <AccountId>11</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Alasdair Firth</DisplayName>
+        <AccountId>30</AccountId>
+        <AccountType/>
+      </UserInfo>
+    </SharedWithUsers>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100AF102A4A1803344B8D888EB900B09227" ma:contentTypeVersion="8" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="43bc291949bcf5a898aed47fdf38e56c">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="090e8724-afd2-4a00-8d2e-c87448cad135" xmlns:ns3="cce065d8-4207-498d-8ddb-77753710233a" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="8a89575b99fa510669e25d545522f68e" ns2:_="" ns3:_="">
     <xsd:import namespace="090e8724-afd2-4a00-8d2e-c87448cad135"/>
@@ -26759,35 +26817,25 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <SharedWithUsers xmlns="cce065d8-4207-498d-8ddb-77753710233a">
-      <UserInfo>
-        <DisplayName>Christine Reid</DisplayName>
-        <AccountId>11</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Alasdair Firth</DisplayName>
-        <AccountId>30</AccountId>
-        <AccountType/>
-      </UserInfo>
-    </SharedWithUsers>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{170C8C87-D947-4550-B837-5AF2D61371C8}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{98190E4F-1B18-40B8-A20A-C34BFF97A2BB}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="cce065d8-4207-498d-8ddb-77753710233a"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E6617C3D-29D9-48EE-BF3C-21AA1A387073}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -26804,22 +26852,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{98190E4F-1B18-40B8-A20A-C34BFF97A2BB}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="cce065d8-4207-498d-8ddb-77753710233a"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{170C8C87-D947-4550-B837-5AF2D61371C8}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>